<commit_message>
[skip netlify] make table lower case
</commit_message>
<xml_diff>
--- a/Other files/Tables For Prod 2.xlsx
+++ b/Other files/Tables For Prod 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A1B8B4-BDDB-41A4-9E95-187D7C2240F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA30B4E0-A6D4-4C52-9F11-C4CB0AC60114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,19 +17,19 @@
     <sheet name="teams" sheetId="1" r:id="rId2"/>
     <sheet name="players" sheetId="3" r:id="rId3"/>
     <sheet name="conferences" sheetId="14" r:id="rId4"/>
-    <sheet name="Roles" sheetId="15" r:id="rId5"/>
-    <sheet name="AnswerTypes" sheetId="17" r:id="rId6"/>
+    <sheet name="roles" sheetId="15" r:id="rId5"/>
+    <sheet name="answertypes" sheetId="17" r:id="rId6"/>
     <sheet name="Users" sheetId="2" r:id="rId7"/>
-    <sheet name="PredictionPeriods" sheetId="4" r:id="rId8"/>
-    <sheet name="Events" sheetId="16" r:id="rId9"/>
+    <sheet name="predictionperiods" sheetId="4" r:id="rId8"/>
+    <sheet name="events" sheetId="16" r:id="rId9"/>
     <sheet name="PeriodPredictions" sheetId="5" r:id="rId10"/>
     <sheet name="PrivateLeagues" sheetId="8" r:id="rId11"/>
     <sheet name="ScoringSettings" sheetId="10" r:id="rId12"/>
     <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId13"/>
     <sheet name="UserScores" sheetId="12" r:id="rId14"/>
-    <sheet name="Franchises" sheetId="18" r:id="rId15"/>
+    <sheet name="franchises" sheetId="18" r:id="rId15"/>
     <sheet name="EmailSubscriptions" sheetId="19" r:id="rId16"/>
-    <sheet name="EmailTypes" sheetId="20" r:id="rId17"/>
+    <sheet name="emailtypes" sheetId="20" r:id="rId17"/>
     <sheet name="Dates" sheetId="21" r:id="rId18"/>
     <sheet name="SQL Commands" sheetId="13" r:id="rId19"/>
   </sheets>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="325">
   <si>
     <t>TeamID</t>
   </si>
@@ -329,9 +329,6 @@
     <t>PredictionPeriodID</t>
   </si>
   <si>
-    <t>KO of Super Bowl LVI</t>
-  </si>
-  <si>
     <t>PP1</t>
   </si>
   <si>
@@ -797,18 +794,9 @@
     <t>KO of 2022 Regular Season opener</t>
   </si>
   <si>
-    <t>KO of 2021 Regular Season opener</t>
-  </si>
-  <si>
     <t>EventDateTimeUTC</t>
   </si>
   <si>
-    <t>Start of 2022 League Year and Free Agency</t>
-  </si>
-  <si>
-    <t>Start of 2022 NFL Draft</t>
-  </si>
-  <si>
     <t>Start of 2023 League Year and Free Agency</t>
   </si>
   <si>
@@ -824,21 +812,9 @@
     <t>KO of 1st game in final round of 2022 Regular Season games</t>
   </si>
   <si>
-    <t>KO of 1st game in final round of 2021 Regular Season games</t>
-  </si>
-  <si>
     <t>HowItWorks</t>
   </si>
   <si>
-    <t>INSERT INTO roles(roleid,name) VALUES(1,'ROLE_USER');</t>
-  </si>
-  <si>
-    <t>INSERT INTO roles(roleid,name) VALUES(2,'ROLE_MODERATOR');</t>
-  </si>
-  <si>
-    <t>INSERT INTO roles(roleid,name) VALUES(3,'ROLE_ADMIN');</t>
-  </si>
-  <si>
     <t>AnswerTypeID</t>
   </si>
   <si>
@@ -866,9 +842,6 @@
     <t>Last Season''s Starter</t>
   </si>
   <si>
-    <t>INSERT INTO the_qb_carousel.answertypes (answertypeid,answertype,answertypetidy) VALUES</t>
-  </si>
-  <si>
     <t>Bryce Young</t>
   </si>
   <si>
@@ -938,9 +911,6 @@
     <t>Nickname2022</t>
   </si>
   <si>
-    <t>INSERT INTO Franchises (FranchiseID, Location2022, Nickname2022) VALUES</t>
-  </si>
-  <si>
     <t>EmailSubscriptionTypeID</t>
   </si>
   <si>
@@ -986,9 +956,6 @@
     <t>Email Verification</t>
   </si>
   <si>
-    <t>INSERT INTO EmailTypes (EmailTypeID,EmailType,Description,EmailTypeTidy,IsSubscription) VALUES</t>
-  </si>
-  <si>
     <t>Dates</t>
   </si>
   <si>
@@ -1068,6 +1035,24 @@
   </si>
   <si>
     <t>Stetson Bennett</t>
+  </si>
+  <si>
+    <t>INSERT INTO roles (roleid,name) VALUES(1,'ROLE_USER');</t>
+  </si>
+  <si>
+    <t>INSERT INTO roles (roleid,name) VALUES(3,'ROLE_ADMIN');</t>
+  </si>
+  <si>
+    <t>INSERT INTO roles (roleid,name) VALUES(2,'ROLE_MODERATOR');</t>
+  </si>
+  <si>
+    <t>INSERT INTO answertypes (answertypeid,answertype,answertypetidy) VALUES</t>
+  </si>
+  <si>
+    <t>INSERT INTO franchises (FranchiseID, Location2022, Nickname2022) VALUES</t>
+  </si>
+  <si>
+    <t>INSERT INTO emailtypes (EmailTypeID,EmailType,Description,EmailTypeTidy,IsSubscription) VALUES</t>
   </si>
 </sst>
 </file>
@@ -1453,10 +1438,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1464,60 +1449,60 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
         <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1525,10 +1510,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" t="s">
         <v>225</v>
-      </c>
-      <c r="B10" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1551,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>80</v>
@@ -1575,7 +1560,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1587,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2A964-6D6F-40DF-AB3E-3D03D24B0F24}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1598,13 +1583,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1615,7 +1600,7 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1637,33 +1622,33 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -1683,10 +1668,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3">
         <v>0.24419428096993967</v>
@@ -1721,7 +1706,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>74</v>
@@ -1740,7 +1725,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1748,7 +1733,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1756,7 +1741,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1785,10 +1770,10 @@
         <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3450,8 +3435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B34627-8194-453E-A9E5-FAABA9941246}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E1:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3463,16 +3448,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>286</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3486,7 +3471,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"'),"</f>
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"')"&amp;IF(LEN(A3)&gt;0,",",";")</f>
         <v>(1,'Baltimore','Ravens'),</v>
       </c>
     </row>
@@ -3501,7 +3486,7 @@
         <v>50</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E33" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"'),"</f>
+        <f t="shared" ref="E3:E33" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"')"&amp;IF(LEN(A4)&gt;0,",",";")</f>
         <v>(2,'Cincinnati','Bengals'),</v>
       </c>
     </row>
@@ -3573,7 +3558,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -3615,7 +3600,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
         <v>55</v>
@@ -3828,7 +3813,7 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -3952,7 +3937,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>(32,'Seattle','Seahawks'),</v>
+        <v>(32,'Seattle','Seahawks');</v>
       </c>
     </row>
   </sheetData>
@@ -3965,9 +3950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC6C2B3-0879-4D8D-928D-DD2F288018F7}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3981,10 +3964,10 @@
         <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -3997,37 +3980,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789449E2-1E71-4639-A31F-FEE451B9A1CF}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4035,19 +4018,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C2" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D2" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;SUBSTITUTE(C2,"'","''")&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;"),"</f>
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;SUBSTITUTE(C2,"'","''")&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;")"&amp;IF(LEN(A3)&gt;0,",",";")</f>
         <v>(1,'EMAILTYPE_PREDICTIONPERIODOPEN','Email sent out just after the prediction period has opened','Prediction Period Open',1),</v>
       </c>
     </row>
@@ -4056,19 +4039,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C3" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;SUBSTITUTE(C3,"'","''")&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;"),"</f>
+        <f t="shared" ref="F3:F5" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;SUBSTITUTE(C3,"'","''")&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;")"&amp;IF(LEN(A4)&gt;0,",",";")</f>
         <v>(2,'EMAILTYPE_PREDICTIONPERIODCLOSE','Email sent out about a week before the prediction period closes','Prediction Period Close',1),</v>
       </c>
     </row>
@@ -4077,19 +4060,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C4" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D4" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="str">
-        <f>"("&amp;A4&amp;",'"&amp;B4&amp;"','"&amp;SUBSTITUTE(C4,"'","''")&amp;"','"&amp;D4&amp;"',"&amp;E4&amp;"),"</f>
+        <f t="shared" si="0"/>
         <v>(3,'EMAILTYPE_EMAILVERIFICATION','Email to verify user''s email after registration','Email Verification',0),</v>
       </c>
     </row>
@@ -4098,20 +4081,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="C5" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="D5" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="str">
-        <f>"("&amp;A5&amp;",'"&amp;B5&amp;"','"&amp;SUBSTITUTE(C5,"'","''")&amp;"','"&amp;D5&amp;"',"&amp;E5&amp;"),"</f>
-        <v>(4,'EMAILTYPE_PASSWORDRESET','Email sent out to reset user''s email','Password Reset',0),</v>
+        <f t="shared" si="0"/>
+        <v>(4,'EMAILTYPE_PASSWORDRESET','Email sent out to reset user''s email','Password Reset',0);</v>
       </c>
     </row>
   </sheetData>
@@ -4135,119 +4118,119 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" t="s">
         <v>306</v>
-      </c>
-      <c r="C3" t="s">
-        <v>319</v>
-      </c>
-      <c r="D3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E3" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D4" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E4" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="C5" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="D5" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E5" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D6" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E6" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C7" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D7" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E7" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="D8" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E8" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="C9" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="D9" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E9" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -4272,8 +4255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4307,19 +4290,19 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="L1" t="str">
         <f>"INSERT INTO teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:J1)&amp;") VALUES"</f>
@@ -4553,7 +4536,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -4658,7 +4641,7 @@
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -5165,7 +5148,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -5570,8 +5553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5585,13 +5568,13 @@
         <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -5603,7 +5586,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5622,7 +5605,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -5641,7 +5624,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5660,7 +5643,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5678,7 +5661,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5696,7 +5679,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5715,7 +5698,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5734,7 +5717,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5753,7 +5736,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -5772,7 +5755,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5791,7 +5774,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -5810,7 +5793,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -5829,7 +5812,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -5848,7 +5831,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -5867,7 +5850,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -5886,7 +5869,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -5905,7 +5888,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -5924,7 +5907,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -5943,7 +5926,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -5962,7 +5945,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -5981,7 +5964,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -6000,7 +5983,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -6019,7 +6002,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -6038,7 +6021,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -6057,7 +6040,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -6076,7 +6059,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -6095,7 +6078,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -6114,7 +6097,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -6133,7 +6116,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -6152,7 +6135,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -6171,7 +6154,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -6190,7 +6173,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -6209,7 +6192,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -6228,7 +6211,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -6247,7 +6230,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -6266,7 +6249,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -6285,7 +6268,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -6304,7 +6287,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -6323,7 +6306,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -6342,7 +6325,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -6361,7 +6344,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -6380,7 +6363,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -6399,7 +6382,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -6418,7 +6401,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -6437,7 +6420,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -6456,7 +6439,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -6475,7 +6458,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -6494,7 +6477,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -6513,7 +6496,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -6532,7 +6515,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -6551,7 +6534,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -6570,7 +6553,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -6589,7 +6572,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -6608,7 +6591,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -6627,7 +6610,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -6646,7 +6629,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -6665,7 +6648,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -6684,7 +6667,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -6703,7 +6686,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -6722,7 +6705,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -6741,7 +6724,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -6760,7 +6743,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -6779,7 +6762,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -6798,7 +6781,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -6817,7 +6800,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -6836,7 +6819,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -6855,7 +6838,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -6874,7 +6857,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -6893,7 +6876,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -6912,7 +6895,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -6931,7 +6914,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -6950,7 +6933,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -6969,7 +6952,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -6988,7 +6971,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -7007,7 +6990,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -7026,7 +7009,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -7045,7 +7028,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -7064,7 +7047,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -7083,7 +7066,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -7102,7 +7085,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -7121,7 +7104,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -7140,7 +7123,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -7159,7 +7142,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -7178,7 +7161,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -7197,7 +7180,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -7216,7 +7199,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -7235,7 +7218,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -7254,7 +7237,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -7273,7 +7256,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -7292,7 +7275,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -7311,7 +7294,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -7330,7 +7313,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -7349,7 +7332,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -7368,7 +7351,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -7387,7 +7370,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -7402,7 +7385,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -7417,7 +7400,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -7432,7 +7415,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -7447,7 +7430,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -7462,7 +7445,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -7477,7 +7460,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -7489,92 +7472,92 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="1"/>
-        <v>(101,'Jaren Hall',1),</v>
+        <v>(102,'Jaren Hall',1),</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="1"/>
-        <v>(101,'Jayden Daniels',1),</v>
+        <v>(103,'Jayden Daniels',1),</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="1"/>
-        <v>(101,'Malik Cunningham',1),</v>
+        <v>(104,'Malik Cunningham',1),</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="1"/>
-        <v>(101,'Spencer Rattler',1),</v>
+        <v>(105,'Spencer Rattler',1),</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="1"/>
-        <v>(101,'Cameron Ward',1),</v>
+        <v>(106,'Cameron Ward',1),</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="1"/>
-        <v>(101,'Stetson Bennett',1);</v>
+        <v>(107,'Stetson Bennett',1);</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -7680,7 +7663,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I1" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7696,29 +7679,29 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I1" t="str" cm="1">
-        <f t="array" aca="1" ref="I1" ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
-        <v>INSERT INTO conferences(ConferenceID,Season,Name,GridColumn,GridRowStart,GridRowEnd,IsActive) VALUES</v>
+        <f t="array" aca="1" ref="I1" ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
+        <v>INSERT INTO conferences (ConferenceID,Season,Name,GridColumn,GridRowStart,GridRowEnd,IsActive) VALUES</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -7744,7 +7727,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="str">
-        <f>"("&amp;A2&amp;","&amp;B2&amp;",'"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <f>"("&amp;A2&amp;","&amp;B2&amp;",'"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;")"&amp;IF(LEN(A3)&gt;0,",",";")</f>
         <v>(1,2023,'AFC',1,2,6,0),</v>
       </c>
     </row>
@@ -7771,8 +7754,8 @@
         <v>0</v>
       </c>
       <c r="I3" t="str">
-        <f>"("&amp;A3&amp;","&amp;B3&amp;",'"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
-        <v>(2,2023,'NFC',1,6,10,0)</v>
+        <f>"("&amp;A3&amp;","&amp;B3&amp;",'"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",",";")</f>
+        <v>(2,2023,'NFC',1,6,10,0);</v>
       </c>
     </row>
   </sheetData>
@@ -7786,7 +7769,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="D4" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7797,10 +7780,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -7808,10 +7791,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D2" t="s">
-        <v>250</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -7819,10 +7802,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D3" t="s">
-        <v>251</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -7830,10 +7813,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -7847,7 +7830,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E4" sqref="E1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7859,16 +7842,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
-        <v>262</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -7876,10 +7859,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E2" t="str">
         <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"')"&amp;IF(LEN(A3)&gt;0,",",";")</f>
@@ -7891,10 +7874,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E3" t="str">
         <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"')"&amp;IF(LEN(A4)&gt;0,",",";")</f>
@@ -7906,10 +7889,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E4" t="str">
         <f>"("&amp;A4&amp;",'"&amp;B4&amp;"','"&amp;C4&amp;"')"&amp;IF(LEN(A5)&gt;0,",",";")</f>
@@ -7950,19 +7933,19 @@
         <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>76</v>
@@ -7979,7 +7962,7 @@
         <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
         <v>79</v>
@@ -7996,7 +7979,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -8012,7 +7995,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8033,26 +8016,26 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="J1" t="str" cm="1">
-        <f t="array" aca="1" ref="J1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:H1)&amp;") VALUES"</f>
-        <v>INSERT INTO the_qb_carousel.PredictionPeriods(PredictionPeriodID,Season,SeasonPeriodID,FromEventID,ToEventID,HowItWorks,IsActive,IsSeasonTotal) VALUES</v>
+        <f t="array" aca="1" ref="J1" ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:H1)&amp;") VALUES"</f>
+        <v>INSERT INTO predictionperiods (PredictionPeriodID,Season,SeasonPeriodID,FromEventID,ToEventID,HowItWorks,IsActive,IsSeasonTotal) VALUES</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -8060,7 +8043,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8081,8 +8064,8 @@
         <v>0</v>
       </c>
       <c r="J2" t="str">
-        <f>"('"&amp;A2&amp;"',"&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"',"&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
-        <v>('1',2022,'1','1','2',1,1,0),</v>
+        <f>"('"&amp;A2&amp;"',"&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;")"&amp;IF(LEN(A3)&gt;0,",",";")</f>
+        <v>('1',2023,1,1,2,1,1,0),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -8090,7 +8073,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8111,8 +8094,8 @@
         <v>0</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J9" si="0">"('"&amp;A3&amp;"',"&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"',"&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
-        <v>('2',2022,'2','2','3',1,1,0),</v>
+        <f t="shared" ref="J3:J9" si="0">"('"&amp;A3&amp;"',"&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;")"&amp;IF(LEN(A4)&gt;0,",",";")</f>
+        <v>('2',2023,2,2,3,1,1,0),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -8120,7 +8103,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8142,7 +8125,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>('3',2022,'3','3','4',1,1,0),</v>
+        <v>('3',2023,3,3,4,1,1,0),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -8150,7 +8133,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -8172,127 +8155,55 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>('4',2022,'4','4','5',1,1,0),</v>
+        <v>('4',2023,4,4,5,1,1,0),</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>1234</v>
       </c>
       <c r="B6">
         <v>2023</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
+        <v>122</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>('5',2023,'1','6','7',0,1,0),</v>
+        <v>('1234',2023,NULL,NULL,NULL,0,0,1);</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2023</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>('6',2023,'2','7','8',0,1,0),</v>
+        <v>('',,,,,,,);</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>2023</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>('7',2023,'3','8','9',0,1,0),</v>
+        <v>('',,,,,,,);</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>2023</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>('8',2023,'4','9','10',0,1,0)</v>
+        <v>('',,,,,,,);</v>
       </c>
     </row>
   </sheetData>
@@ -8303,10 +8214,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F502399-C795-4D5E-88DC-92C8B5181153}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8319,20 +8230,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="F1" t="str" cm="1">
-        <f t="array" aca="1" ref="F1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
-        <v>INSERT INTO the_qb_carousel.Events(EventID,EventName,EventDateTimeUTC,DateConfirmed) VALUES</v>
+        <f t="array" aca="1" ref="F1" ca="1">"INSERT INTO "&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;" ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
+        <v>INSERT INTO events (EventID,EventName,EventDateTimeUTC,DateConfirmed) VALUES</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -8340,17 +8251,17 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C2" s="3">
-        <v>44449.013888888891</v>
+        <v>44813.013888888891</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"',"&amp;IF(LEN(C2)&gt;0,"'"&amp;TEXT(C2,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
-        <v>(1,'KO of 2021 Regular Season opener','2021-09-10 00:20',1),</v>
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"',"&amp;IF(LEN(C2)&gt;0,"'"&amp;TEXT(C2,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D2&amp;")"&amp;IF(LEN(A3)&gt;0,",",";")</f>
+        <v>(1,'KO of 2022 Regular Season opener','2022-09-09 00:20',1),</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -8358,17 +8269,17 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C3" s="3">
-        <v>44569.895833333336</v>
+        <v>44933.895833333336</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F16" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"',"&amp;IF(LEN(C3)&gt;0,"'"&amp;TEXT(C3,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
-        <v>(2,'KO of 1st game in final round of 2021 Regular Season games','2022-01-08 21:30',1),</v>
+        <f t="shared" ref="F3:F16" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"',"&amp;IF(LEN(C3)&gt;0,"'"&amp;TEXT(C3,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D3&amp;")"&amp;IF(LEN(A4)&gt;0,",",";")</f>
+        <v>(2,'KO of 1st game in final round of 2022 Regular Season games','2023-01-07 21:30',1),</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -8376,17 +8287,17 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C4" s="3">
-        <v>44605.979166666664</v>
+        <v>44969.979166666664</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>(3,'KO of Super Bowl LVI','2022-02-13 23:30',1),</v>
+        <v>(3,'KO of Super Bowl LVII','2023-02-12 23:30',1),</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -8394,17 +8305,17 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C5" s="3">
-        <v>44636.833333333336</v>
+        <v>45000.833333333336</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>(4,'Start of 2022 League Year and Free Agency','2022-03-16 20:00',1),</v>
+        <v>(4,'Start of 2023 League Year and Free Agency','2023-03-15 20:00',1),</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -8412,17 +8323,17 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C6" s="3">
-        <v>44680</v>
+        <v>45044</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>(5,'Start of 2022 NFL Draft','2022-04-29 00:00',1),</v>
+        <v>(5,'Start of 2023 NFL Draft','2023-04-28 00:00',1),</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -8430,17 +8341,17 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="C7" s="3">
-        <v>44813.013888888891</v>
+        <v>45177.013888888891</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>(6,'KO of 2022 Regular Season opener','2022-09-09 00:20',1),</v>
+        <v>(6,'KO of 2023 Regular Season opener','2023-09-08 00:20',0),</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -8448,17 +8359,17 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="C8" s="3">
-        <v>44935.895833333336</v>
+        <v>45298.895833333336</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>(7,'KO of 1st game in final round of 2022 Regular Season games','2023-01-09 21:30',0),</v>
+        <v>(7,'KO of 1st game in final round of 2023 Regular Season games','2024-01-07 21:30',0),</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -8466,17 +8377,17 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>271</v>
       </c>
       <c r="C9" s="3">
-        <v>44969.979166666664</v>
+        <v>45333.979166666664</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>(8,'KO of Super Bowl LVII','2023-02-12 23:30',1),</v>
+        <v>(8,'KO of Super Bowl LVIII','2024-02-11 23:30',0),</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -8484,17 +8395,17 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="C10" s="3">
-        <v>45000.833333333336</v>
+        <v>45365.833333333336</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>(9,'Start of 2023 League Year and Free Agency','2023-03-15 20:00',1),</v>
+        <v>(9,'Start of 2024 League Year and Free Agency','2024-03-14 20:00',0),</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -8502,108 +8413,98 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="C11" s="3">
-        <v>45044</v>
+        <v>45408</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>(10,'Start of 2023 NFL Draft','2023-04-28 00:00',1),</v>
+        <v>(10,'Start of 2024 NFL Draft','2024-04-26 00:00',0);</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C12" s="3">
-        <v>45177.013888888891</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>(11,'KO of 2023 Regular Season opener','2023-09-08 00:20',0),</v>
+        <v>(,'',NULL,);</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>277</v>
-      </c>
-      <c r="C13" s="3">
-        <v>45298.895833333336</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>(12,'KO of 1st game in final round of 2023 Regular Season games','2024-01-07 21:30',0),</v>
+        <v>(,'',NULL,);</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C14" s="3">
-        <v>45333.979166666664</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>(13,'KO of Super Bowl LVIII','2024-02-11 23:30',0),</v>
+        <v>(,'',NULL,);</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>278</v>
-      </c>
-      <c r="C15" s="3">
-        <v>45365.833333333336</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>(14,'Start of 2024 League Year and Free Agency','2024-03-14 20:00',0),</v>
+        <v>(,'',NULL,);</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>279</v>
-      </c>
-      <c r="C16" s="3">
-        <v>45408</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>(15,'Start of 2024 NFL Draft','2024-04-26 00:00',0)</v>
-      </c>
+        <v>(,'',NULL,);</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>